<commit_message>
Workbook save for 03/22 meeting
</commit_message>
<xml_diff>
--- a/results_beta_V2/RunningDrugDeck_V1_AddBetaV2_CheckDrugCoverage_Cleaned2_032121_WORKBOOK.xlsx
+++ b/results_beta_V2/RunningDrugDeck_V1_AddBetaV2_CheckDrugCoverage_Cleaned2_032121_WORKBOOK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/blucher/git/The-Cancer-Targetome/results_beta_V2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{06FC0DB7-E9DA-9947-9555-0778D1A0E5F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{AEBD82F1-DEB0-CF4F-A6E4-8C1AC71DB4B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="1580" windowWidth="31100" windowHeight="18740"/>
+    <workbookView xWindow="2020" yWindow="640" windowWidth="34520" windowHeight="20720"/>
   </bookViews>
   <sheets>
     <sheet name="RunningDrugDeck_V1_AddBetaV2_Ch" sheetId="1" r:id="rId1"/>
@@ -3397,7 +3397,7 @@
   <dimension ref="A1:H417"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>